<commit_message>
Aggiornate curve di urgenza ed analisi sito esistente
</commit_message>
<xml_diff>
--- a/CurvaDiUrgenza(1).xlsx
+++ b/CurvaDiUrgenza(1).xlsx
@@ -86,9 +86,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.8512580277772673E-2"/>
-          <c:y val="4.9276630130819489E-2"/>
-          <c:w val="0.86134389912183618"/>
+          <c:x val="0.13621834975191024"/>
+          <c:y val="4.9276752007648077E-2"/>
+          <c:w val="0.80227964605062463"/>
           <c:h val="0.69304152042663314"/>
         </c:manualLayout>
       </c:layout>
@@ -99,7 +99,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Semplicità</c:v>
+            <c:v>Visibilità stato Sistema</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575">
@@ -113,7 +113,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -125,7 +125,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -136,7 +136,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Gerarchia Visiva</c:v>
+            <c:v>Match Sistema-Mondo Reale</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575">
@@ -150,7 +150,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -162,7 +162,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -173,7 +173,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Navigabilità</c:v>
+            <c:v>User Control e Libertà</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575">
@@ -210,7 +210,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>Consistenza</c:v>
+            <c:v>Coerenze e Standard</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575">
@@ -224,7 +224,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -236,7 +236,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -251,13 +251,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="198955392"/>
-        <c:axId val="198957312"/>
+        <c:axId val="211403520"/>
+        <c:axId val="211405440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="198955392"/>
+        <c:axId val="211403520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="6"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -285,14 +286,15 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198957312"/>
+        <c:crossAx val="211405440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="198957312"/>
+        <c:axId val="211405440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="6"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -328,7 +330,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198955392"/>
+        <c:crossAx val="211403520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -372,13 +374,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>124483</xdr:colOff>
+      <xdr:colOff>124481</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>168822</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>578069</xdr:colOff>
+      <xdr:colOff>581024</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>26276</xdr:rowOff>
     </xdr:to>
@@ -406,12 +408,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.07431</cdr:x>
-      <cdr:y>0.16503</cdr:y>
+      <cdr:x>0.11971</cdr:x>
+      <cdr:y>0.16292</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.23339</cdr:x>
-      <cdr:y>0.16503</cdr:y>
+      <cdr:x>0.26914</cdr:x>
+      <cdr:y>0.16292</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
@@ -420,8 +422,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="351489" y="573785"/>
-          <a:ext cx="752425" cy="0"/>
+          <a:off x="564249" y="566475"/>
+          <a:ext cx="704350" cy="0"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
@@ -494,7 +496,7 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.65809</cdr:x>
+      <cdr:x>0.67154</cdr:x>
       <cdr:y>0.62833</cdr:y>
     </cdr:from>
     <cdr:to>
@@ -508,8 +510,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="3112757" y="2184679"/>
-          <a:ext cx="704140" cy="0"/>
+          <a:off x="3165307" y="2184675"/>
+          <a:ext cx="638287" cy="0"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
@@ -538,7 +540,7 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.51684</cdr:x>
+      <cdr:x>0.53786</cdr:x>
       <cdr:y>0.51286</cdr:y>
     </cdr:from>
     <cdr:to>
@@ -552,8 +554,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2444658" y="1783174"/>
-          <a:ext cx="695635" cy="0"/>
+          <a:off x="2535192" y="1783191"/>
+          <a:ext cx="594138" cy="0"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
@@ -582,11 +584,11 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.37421</cdr:x>
+      <cdr:x>0.40418</cdr:x>
       <cdr:y>0.3959</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.5167</cdr:x>
+      <cdr:x>0.53475</cdr:x>
       <cdr:y>0.3959</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
@@ -596,8 +598,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1769988" y="1376513"/>
-          <a:ext cx="673995" cy="0"/>
+          <a:off x="1905077" y="1376526"/>
+          <a:ext cx="615461" cy="0"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
@@ -626,11 +628,11 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.2274</cdr:x>
+      <cdr:x>0.26894</cdr:x>
       <cdr:y>0.28083</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.37504</cdr:x>
+      <cdr:x>0.40613</cdr:x>
       <cdr:y>0.28083</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
@@ -640,8 +642,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1075614" y="976421"/>
-          <a:ext cx="698334" cy="0"/>
+          <a:off x="1267634" y="976433"/>
+          <a:ext cx="646650" cy="0"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
@@ -670,11 +672,11 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.66095</cdr:x>
+      <cdr:x>0.67028</cdr:x>
       <cdr:y>0.51381</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.66095</cdr:x>
+      <cdr:x>0.67028</cdr:x>
       <cdr:y>0.62781</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
@@ -684,8 +686,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="3126273" y="1786477"/>
-          <a:ext cx="0" cy="396391"/>
+          <a:off x="3159339" y="1786494"/>
+          <a:ext cx="0" cy="396372"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
@@ -714,11 +716,11 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.51692</cdr:x>
+      <cdr:x>0.53402</cdr:x>
       <cdr:y>0.39414</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.51692</cdr:x>
+      <cdr:x>0.53402</cdr:x>
       <cdr:y>0.51256</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
@@ -728,7 +730,7 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2445035" y="1370420"/>
+          <a:off x="2517091" y="1370407"/>
           <a:ext cx="0" cy="411741"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
@@ -758,12 +760,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.3745</cdr:x>
-      <cdr:y>0.27867</cdr:y>
+      <cdr:x>0.40403</cdr:x>
+      <cdr:y>0.28288</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.3745</cdr:x>
-      <cdr:y>0.39354</cdr:y>
+      <cdr:x>0.40403</cdr:x>
+      <cdr:y>0.39775</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
@@ -772,8 +774,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1771402" y="968916"/>
-          <a:ext cx="0" cy="399400"/>
+          <a:off x="1904412" y="983577"/>
+          <a:ext cx="0" cy="399397"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
@@ -802,12 +804,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.22898</cdr:x>
-      <cdr:y>0.16682</cdr:y>
+      <cdr:x>0.2694</cdr:x>
+      <cdr:y>0.16471</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.22898</cdr:x>
-      <cdr:y>0.28207</cdr:y>
+      <cdr:x>0.2694</cdr:x>
+      <cdr:y>0.27996</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
@@ -816,8 +818,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1083078" y="580040"/>
-          <a:ext cx="0" cy="400707"/>
+          <a:off x="1269794" y="572698"/>
+          <a:ext cx="0" cy="400719"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
@@ -1136,26 +1138,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1168,10 +1170,10 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>